<commit_message>
Another Major Update (see Description)
- Reconfigured Ballast Gearing Arrangement to account for new gear pitch spacing
- Also slightly shifted the bearing and thrust distributor to account for new gear dimensions
- Added hall effect sensors to both spool shafts and the drive shaft (and removed phototransistors where applicable)
- Added magnet mounts (and respective shaft collars) to every shaft
- Added 4th Arduino Nano for the spool carrage encoder
- Generated final DXF Files of the Sealing discs for waterjet
- Extended small spool length/carrage shaft lengths
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2DD89-0D5C-494E-A83D-43816133EB78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C4034-1221-40EF-8323-25ADA570AB5F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>Mcmaster</t>
+  </si>
+  <si>
+    <t>Compleat Sculptor</t>
+  </si>
+  <si>
+    <t>XTC Smooth-On Epoxy Die</t>
+  </si>
+  <si>
+    <t>The Compleat Sculptor</t>
+  </si>
+  <si>
+    <t>Waterjet Order</t>
+  </si>
+  <si>
+    <t>5 Sealing Discs Waterjet Order</t>
+  </si>
+  <si>
+    <t>RPI MILL</t>
   </si>
 </sst>
 </file>
@@ -144,15 +162,15 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -472,7 +490,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,298 +498,320 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <f>SUM(E3:E39)</f>
-        <v>155</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>42628</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>42842</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>43042</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>43056</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
+        <v>43151</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>43194</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>43194</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="2"/>
-    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="4">
+        <v>43202</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="2"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="2"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="2"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="2"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="2"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="2"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="2"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
+      <c r="E34" s="1"/>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="2"/>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="2"/>
+      <c r="E36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Minor Changes to Pinout, final assembly
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C4034-1221-40EF-8323-25ADA570AB5F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECF5724-5527-452E-8D3D-72C6F10B8B57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +536,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(E3:E39)</f>
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Another Major Update - See Description
- Updated DC Motor model with proper dimensions
- Updated Gear models - added teeth to those without, adjusted dimensions, added Teeth/pitch emboss
- Updated Threaded Rod lengths with proper lengths post-machining
- Completed proper motion-translation constraints of the ballast system - piston now moves in time with the gear train, with proper teeth correction!
- Front servo plate/cover modified, screws removed as they were not necessary
- Ballast Gear train updated- new gear teeth combos used, models updated, standoffs and axles expanded in length to accomidate changes
- Other minor Adjustments/Updates
- cost breakdown updated
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECF5724-5527-452E-8D3D-72C6F10B8B57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE7DFCB-98A7-4E68-9EED-16DBAEB8B8C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>RPI MILL</t>
+  </si>
+  <si>
+    <t>Additional Aluminum, Threaded Rods, Nuts, Wiring Tubing</t>
+  </si>
+  <si>
+    <t>Amazon Motor Order</t>
+  </si>
+  <si>
+    <t>DC Brushed Motor 80T</t>
+  </si>
+  <si>
+    <t>Amazon</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +548,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(E3:E39)</f>
-        <v>180</v>
+        <v>252.14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,17 +687,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="1"/>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>43206</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1">
+        <v>57.14</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="4">
+        <v>43211</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>

</xml_diff>

<commit_message>
Updated Cost Breakdown (WIP), Updated Motor Assembly and Final Assy
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE7DFCB-98A7-4E68-9EED-16DBAEB8B8C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E92ACB5-2A5C-4B7A-9B6F-05F5618105D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -118,6 +119,147 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>Submarine Remaining Parts</t>
+  </si>
+  <si>
+    <t>Add. Notes</t>
+  </si>
+  <si>
+    <t>200mm long 4mm Diameter shaft</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-200mm-Length-Round-Shaft/dp/B01N1LUCH7/ref=sr_1_5?ie=UTF8&amp;qid=1529253512&amp;sr=8-5&amp;keywords=4mm+shaft+200mm</t>
+  </si>
+  <si>
+    <t>4mm Ball Bearing</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#7804k129/=1dew8kd</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Total Price W/O Shipping</t>
+  </si>
+  <si>
+    <t>Needs M4 Die to add thread</t>
+  </si>
+  <si>
+    <t>shipping estimated.</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Airplane-Stainless-Steel-Round-Axles/dp/B00OK42ZOG/ref=sr_1_10?ie=UTF8&amp;qid=1529786532&amp;sr=8-10&amp;keywords=3mm+shaft</t>
+  </si>
+  <si>
+    <t>3mm shaft (5pack) for all control surfaces</t>
+  </si>
+  <si>
+    <t>3mm bushings</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#6658k64/=1dewj1f</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Rudder-Yoke-L5.html</t>
+  </si>
+  <si>
+    <t>Control Yokes 3mm</t>
+  </si>
+  <si>
+    <t>300mm long 2mm diameter threaded push rods (2 pack)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-Airplane-Parts-Threaded-Length/dp/B01LBJKQZW/ref=sr_1_47?ie=UTF8&amp;qid=1529789116&amp;sr=8-47&amp;keywords=2mm+rod</t>
+  </si>
+  <si>
+    <t>Thread class unknown</t>
+  </si>
+  <si>
+    <t>2mm clevises (pack of 5)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Threaded-Metal-Clevis-2x25mm-Airplane/dp/B00XBGKIKC/ref=sr_1_3?ie=UTF8&amp;qid=1529788008&amp;sr=8-3&amp;keywords=clevis+2mm&amp;dpID=41IfImQMKkL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>Need to check push rod thread for compatibility</t>
+  </si>
+  <si>
+    <t>Push Rod Seals, 2mm</t>
+  </si>
+  <si>
+    <t>Push Rod Seals, 3mm</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Pushrod-Seals/Pushrod-Seal-2-mm.html?listtype=search&amp;searchparam=push</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Pushrod-Seals/Pushrod-Seal-3-mm.html</t>
+  </si>
+  <si>
+    <t>Bolt, Button Head, 5-40 thread, 1inch long</t>
+  </si>
+  <si>
+    <t>4mm shaft seal</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Shaft-Sealing-Ring-4-11-6-for-shaft-4mm.html?listtype=search&amp;searchparam=seal</t>
+  </si>
+  <si>
+    <t>540 Motor Mount</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Motor-Mount-540.html</t>
+  </si>
+  <si>
+    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Couplings/Coupler-3-17-4mm.html</t>
+  </si>
+  <si>
+    <t>Motor Coupling</t>
+  </si>
+  <si>
+    <t>DC Motor 80T</t>
+  </si>
+  <si>
+    <t>estimated. Might be able to use an old one</t>
+  </si>
+  <si>
+    <t>Motor countroller</t>
+  </si>
+  <si>
+    <t>HS-82MG servo</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Hitec-32082S-HS-82MG-Metal-Micro/dp/B0012YXRJE/ref=sr_1_1?ie=UTF8&amp;qid=1529793545&amp;sr=8-1&amp;keywords=hs-82mg&amp;dpID=41yo3iH-O%252BL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>Servo Shaft Coupler</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Spline-Servo-Shaft-Coupler-Screw/dp/B00KRJ6MA6/ref=sr_1_2?ie=UTF8&amp;qid=1529794225&amp;sr=8-2&amp;keywords=servo+shaft+coupler&amp;dpID=316JMPzK3BL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>.125" ID Bushing</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#6391k113/=1dey23w</t>
   </si>
 </sst>
 </file>
@@ -501,20 +643,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7607A2C9-437F-4FE2-AFDA-0D0C0CE9A3E2}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -527,7 +669,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -551,7 +693,7 @@
         <v>252.14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>42628</v>
       </c>
@@ -568,7 +710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>42842</v>
       </c>
@@ -585,7 +727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43042</v>
       </c>
@@ -602,7 +744,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43056</v>
       </c>
@@ -619,7 +761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43151</v>
       </c>
@@ -636,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43194</v>
       </c>
@@ -653,7 +795,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43194</v>
       </c>
@@ -670,7 +812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43202</v>
       </c>
@@ -687,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43206</v>
       </c>
@@ -704,7 +846,7 @@
         <v>57.14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43211</v>
       </c>
@@ -721,130 +863,130 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
     </row>
   </sheetData>
@@ -854,4 +996,834 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.12</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3*C3</f>
+        <v>4.12</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3+E3</f>
+        <v>4.12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.31</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E44" si="0">D4*C4</f>
+        <v>8.31</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G44" si="1">F4+E4</f>
+        <v>11.31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6.26</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.26</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.38</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>10.379999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>40.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>45.5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.99</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>4.99</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.63</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.63</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>4.63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000005</v>
+      </c>
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Main Assy, needs new or replacement parts added (WIP). Updated Cost Spreadsheet
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Submarine-project\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E92ACB5-2A5C-4B7A-9B6F-05F5618105D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA55B7DC-8E1B-485E-90D5-4F2A84B60BD0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SERVO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -244,22 +245,79 @@
     <t>Motor countroller</t>
   </si>
   <si>
-    <t>HS-82MG servo</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Hitec-32082S-HS-82MG-Metal-Micro/dp/B0012YXRJE/ref=sr_1_1?ie=UTF8&amp;qid=1529793545&amp;sr=8-1&amp;keywords=hs-82mg&amp;dpID=41yo3iH-O%252BL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>Servo Shaft Coupler</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Spline-Servo-Shaft-Coupler-Screw/dp/B00KRJ6MA6/ref=sr_1_2?ie=UTF8&amp;qid=1529794225&amp;sr=8-2&amp;keywords=servo+shaft+coupler&amp;dpID=316JMPzK3BL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
     <t>.125" ID Bushing</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/#6391k113/=1dey23w</t>
+  </si>
+  <si>
+    <t>.125" shaft</t>
+  </si>
+  <si>
+    <t>need 22 inches total</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#1257k39/=1dfcnqq</t>
+  </si>
+  <si>
+    <t>Encoder magnets</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#5862k13/=1cd8mhi</t>
+  </si>
+  <si>
+    <t>HS 82MG</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>Free Speed (RPM)</t>
+  </si>
+  <si>
+    <t>Stall Torque (Kg-cm)</t>
+  </si>
+  <si>
+    <t>Actual Carriage Travel Speed (inches/second):</t>
+  </si>
+  <si>
+    <t>Actual Spool Rotation Rate (Rev/Sec):</t>
+  </si>
+  <si>
+    <t>HS 645MG</t>
+  </si>
+  <si>
+    <t>Need around/at least 3 kg-cm torque for spool drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEEP SPOOL SERVO (Use Hex insert nut into 3d printed part, attaches to horn). </t>
+  </si>
+  <si>
+    <t>REPLACE CARRAGE SERVO (Use gear motor with 3mm output shaft, use 3mm shaft coupler listed below, already ordered).</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SODIAL-Aluminum-Flexible-Coupling-Connector/dp/B072KRCMJS/ref=sr_1_10?s=hi&amp;ie=UTF8&amp;qid=1529867349&amp;sr=1-10&amp;keywords=3mm%2Bshaft%2Bcoupler&amp;th=1</t>
+  </si>
+  <si>
+    <t>3mm-3mm shaft coupler</t>
+  </si>
+  <si>
+    <t>DC Gear Motor 71RPM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0719DL1J4/ref=oh_aui_detailpage_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Spool Carriage</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B072KRCMJS/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Needs .125" hole in one end for shaft mate</t>
+  </si>
+  <si>
+    <t>TOTAL COST</t>
   </si>
 </sst>
 </file>
@@ -647,16 +705,16 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -669,7 +727,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -693,7 +751,7 @@
         <v>252.14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>42628</v>
       </c>
@@ -710,7 +768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>42842</v>
       </c>
@@ -727,7 +785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43042</v>
       </c>
@@ -744,7 +802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43056</v>
       </c>
@@ -761,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43151</v>
       </c>
@@ -778,7 +836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43194</v>
       </c>
@@ -795,7 +853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43194</v>
       </c>
@@ -812,7 +870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43202</v>
       </c>
@@ -829,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43206</v>
       </c>
@@ -846,7 +904,7 @@
         <v>57.14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43211</v>
       </c>
@@ -863,130 +921,130 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
     </row>
   </sheetData>
@@ -1000,23 +1058,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1025,7 +1084,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1050,9 +1109,15 @@
       <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="2">
+        <f>SUM(G3:G68)</f>
+        <v>213.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1081,7 +1146,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1109,7 +1174,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1134,7 +1199,7 @@
         <v>6.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1162,7 +1227,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1190,7 +1255,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1218,7 +1283,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1246,7 +1311,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1274,7 +1339,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1302,7 +1367,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1322,32 +1387,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1375,7 +1443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1403,7 +1471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -1428,7 +1496,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1453,62 +1521,68 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>20</v>
+        <v>8.77</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>D18*C18</f>
+        <v>8.77</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <f>F18+E18</f>
+        <v>8.77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>5</v>
+        <v>1.88</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.88</v>
       </c>
       <c r="F19" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1531,43 +1605,63 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="1"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6.58</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>13.16</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D22" s="1"/>
+        <v>17.16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.48</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>4.8</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>6.8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
@@ -1579,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
@@ -1591,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
@@ -1603,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
@@ -1615,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
@@ -1627,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
@@ -1639,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
@@ -1651,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
@@ -1663,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
@@ -1675,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
@@ -1687,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
@@ -1699,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
@@ -1711,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
@@ -1723,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
@@ -1735,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
@@ -1747,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
@@ -1759,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
@@ -1771,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
@@ -1783,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
@@ -1795,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1">
         <f t="shared" si="0"/>
@@ -1807,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1">
         <f t="shared" si="0"/>
@@ -1826,4 +1920,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC903C9-CFA0-4037-BB87-4B6ADFD60728}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>2.8</v>
+      </c>
+      <c r="H4">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11">
+        <f>(B3/60)*0.4571*0.1</f>
+        <v>5.3328333333333339E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12">
+        <f>(H3/60)*(31/90)</f>
+        <v>0.22962962962962963</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assembly Changes, Cost breakdown Update, Fixed aft section (WIP)
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA55B7DC-8E1B-485E-90D5-4F2A84B60BD0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B547E6-812F-4F08-BA14-BF1DAE358EFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="150">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Amazon ESC Order</t>
   </si>
   <si>
-    <t>QUICRUN 2060 ESC</t>
-  </si>
-  <si>
     <t>Amazon Filament Order</t>
   </si>
   <si>
@@ -318,6 +315,168 @@
   </si>
   <si>
     <t>TOTAL COST</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#6391k126/=1dfi0m4</t>
+  </si>
+  <si>
+    <t>.25" bushings</t>
+  </si>
+  <si>
+    <t>.25" diameter 5" long spool shaft</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#1257k115/=1dfi12u</t>
+  </si>
+  <si>
+    <t>Bolt, Button Head, 5-40 thread, .625" long</t>
+  </si>
+  <si>
+    <t>Could also use .875"</t>
+  </si>
+  <si>
+    <t>Ballast Tank Threaded Rod (5/16-18 thread)</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#90611a400/=1dfi2y2</t>
+  </si>
+  <si>
+    <t>Screw-Mount Nut (5/16-18) For Ballast Tank (25count)</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#98752a523/=1dfi7du</t>
+  </si>
+  <si>
+    <t>28T Pinion Gear (2count)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/TOOGOO-3-175mm-Pinion-Brushed-Brushless/dp/B075FN58G6/ref=sr_1_54?ie=UTF8&amp;qid=1529888786&amp;sr=8-54&amp;keywords=28t+pinion+gear</t>
+  </si>
+  <si>
+    <t>Long Shipping time</t>
+  </si>
+  <si>
+    <t>16T Pinion Gear 48P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Traxxas-2416-16T-Pinion-Gear/dp/B000XQ2KTU/ref=sr_1_4?ie=UTF8&amp;qid=1529889119&amp;sr=8-4&amp;keywords=16T+pinion+gear+set</t>
+  </si>
+  <si>
+    <t>Check Other sites for better pricing (bulk)</t>
+  </si>
+  <si>
+    <t>M3 8mm SHCS Low Head</t>
+  </si>
+  <si>
+    <t>Ballast Thrust Bearing</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#5906k513/=1cyvllx</t>
+  </si>
+  <si>
+    <t>.125" Bearing (.25" OD, 10 count)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/125x-250x-109-Precision-Bearings-Metal-Shields/dp/B00X8KXAFG/ref=sr_1_4?ie=UTF8&amp;qid=1523395530&amp;sr=8-4&amp;keywords=ball+bearings+1%2F8+1%2F4&amp;dpID=41aeoNIanLL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>For Ballast Gear Train, Spool Carriage Threaded Rod</t>
+  </si>
+  <si>
+    <t>5V 10A Buck Converter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Castle-Creations-Bec-Switching-Regulator/dp/B000MXAR12/ref=sr_1_1?ie=UTF8&amp;qid=1529889704&amp;sr=8-1&amp;keywords=BEC+10A</t>
+  </si>
+  <si>
+    <t>Maybe find one cheaper? Need 10A though</t>
+  </si>
+  <si>
+    <t>16 Channel PWM Driver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HiLetgo-PCA9685-Channel-12-Bit-Arduino/dp/B01D1D0CX2/ref=sr_1_2?ie=UTF8&amp;qid=1529890412&amp;sr=8-2&amp;keywords=servo+driver+board&amp;dpID=511228KD6JL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>For all PWM (servos, LEDs, etc)</t>
+  </si>
+  <si>
+    <t>Arduino Nano 5 Pack</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B01N7I0W77/ref=sxbs_sxwds-stppvp_3?pf_rd_m=ATVPDKIKX0DER&amp;pf_rd_p=6297546923292665688&amp;pd_rd_wg=ddHdE&amp;pf_rd_r=SXBWPAFRVYFKDFR5S237&amp;pf_rd_s=desktop-sx-bottom-slot&amp;pf_rd_t=301&amp;pd_rd_i=B01N7I0W77&amp;pd_rd_w=GY6XU&amp;pf_rd_i=arduino+nano+5+pack&amp;pd_rd_r=3a7c9f18-fd3d-491b-86c9-19ec55cea102&amp;ie=UTF8&amp;qid=1529890713&amp;sr=3#customerReviews</t>
+  </si>
+  <si>
+    <t>Look around for better bulk pricing if need be (unsoldered only)</t>
+  </si>
+  <si>
+    <t>5V Relay 5 Pack</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/WINGONEER-KY-019-Channel-Module-arduino/dp/B06XHJ2PBJ/ref=sr_1_3?ie=UTF8&amp;qid=1529890983&amp;sr=8-3&amp;keywords=5V+relay&amp;dpID=51AfIoxmEZL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
+  </si>
+  <si>
+    <t>Maybe don't need, use existing relays with BJT circuit</t>
+  </si>
+  <si>
+    <t>11.1V Drive Battery 5500mAh</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/FLOUREON-5500mAh-Quadcopter-Airplane-Helicopter/dp/B072HQ47ZL/ref=sr_1_9?ie=UTF8&amp;qid=1517350605&amp;sr=8-9&amp;keywords=11.1v%2Blipo%2Bbattery&amp;th=1</t>
+  </si>
+  <si>
+    <t>Check before ordering that this is correct, (maybe use smaller lower capacity unit?)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/MELASTA-1500mAh-Battery-m4-fpv250-Shredder/dp/B01MZ3IORY/ref=sr_1_7?ie=UTF8&amp;qid=1518731145&amp;sr=8-7&amp;keywords=11.1v+lipo+1500mah</t>
+  </si>
+  <si>
+    <t>Find single battery listing to save $$</t>
+  </si>
+  <si>
+    <t>11.1V electronics Battery 1500mAh (2 pack, only need 1 though)</t>
+  </si>
+  <si>
+    <t>Pressure Transducer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Eyourlife-Universal-Pressure-Transducer-Solenoid/dp/B00RCPDKDA/ref=sr_1_5?ie=UTF8&amp;qid=1519406024&amp;sr=8-5&amp;keywords=pressure%2Bsensor&amp;dpID=41dmeKyEbLL&amp;preST=_SY300_QL70_&amp;dpSrc=srch&amp;th=1</t>
+  </si>
+  <si>
+    <t>Check before ordering</t>
+  </si>
+  <si>
+    <t>Electronics Battery Oring</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#9557k134/=1bkj08p</t>
+  </si>
+  <si>
+    <t>NOT INCLUDED SO FAR:</t>
+  </si>
+  <si>
+    <t>Some Bolts/Nuts (some aren't listed or priced in yet)</t>
+  </si>
+  <si>
+    <t>Tether Wire</t>
+  </si>
+  <si>
+    <t>Radio Equipment</t>
+  </si>
+  <si>
+    <t>Any additional Mini Sub Stuff</t>
+  </si>
+  <si>
+    <t>Possible Propeller, if 3D print doesn't work out</t>
+  </si>
+  <si>
+    <t>Any additional electronics not accounted for</t>
+  </si>
+  <si>
+    <t>Maybe shaft collar(s)</t>
+  </si>
+  <si>
+    <t>QUICRUN 1060 ESC</t>
   </si>
 </sst>
 </file>
@@ -702,7 +861,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,10 +932,10 @@
         <v>42842</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
@@ -790,10 +949,10 @@
         <v>43042</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
@@ -810,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -824,13 +983,13 @@
         <v>43151</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>25</v>
@@ -841,10 +1000,10 @@
         <v>43194</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -858,13 +1017,13 @@
         <v>43194</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>36</v>
@@ -875,13 +1034,13 @@
         <v>43202</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -892,13 +1051,13 @@
         <v>43206</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1">
         <v>57.14</v>
@@ -909,13 +1068,13 @@
         <v>43211</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="1">
         <v>15</v>
@@ -1058,15 +1217,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
@@ -1077,7 +1236,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1086,43 +1245,43 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(G3:G68)</f>
-        <v>213.4</v>
+        <v>435.52000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1142,16 +1301,16 @@
         <v>4.12</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1171,15 +1330,15 @@
         <v>11.31</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1201,10 +1360,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1224,15 +1383,15 @@
         <v>10.379999999999999</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1252,15 +1411,15 @@
         <v>45.5</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1280,15 +1439,15 @@
         <v>4.99</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1308,15 +1467,15 @@
         <v>4.63</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1336,15 +1495,15 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1364,12 +1523,12 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1386,13 +1545,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
         <v>63</v>
-      </c>
-      <c r="B13" t="s">
-        <v>64</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1412,15 +1574,15 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
         <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1440,15 +1602,15 @@
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1468,12 +1630,12 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1493,12 +1655,12 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1518,15 +1680,15 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
         <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>92</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1546,15 +1708,15 @@
         <v>8.77</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1574,15 +1736,15 @@
         <v>1.88</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
         <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>73</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1602,15 +1764,15 @@
         <v>7.6000000000000005</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1630,15 +1792,15 @@
         <v>17.16</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
         <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1658,22 +1820,72 @@
         <v>6.8</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="H23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5.01</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>5.01</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
@@ -1686,54 +1898,124 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4.9800000000000004</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7.77</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>7.77</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.77</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
+      <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.56</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>7.12</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5.12</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>15.36</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.36</v>
+      </c>
+      <c r="H29" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
@@ -1746,126 +2028,276 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="1"/>
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.96</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>1.92</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.5</v>
+      </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.42</v>
+      </c>
+      <c r="H31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="1"/>
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9.49</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>9.49</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
+        <v>9.49</v>
+      </c>
+      <c r="H32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>21.76</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>21.76</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="1"/>
+        <v>21.76</v>
+      </c>
+      <c r="H33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6.99</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>6.99</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="1"/>
+        <v>6.99</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>20</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>10</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="H36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>44</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="H37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>27</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="H38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>19</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7.86</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>7.86</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3</v>
+      </c>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+        <v>10.86</v>
+      </c>
+      <c r="H40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
@@ -1877,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
@@ -1889,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1">
         <f t="shared" si="0"/>
@@ -1901,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1">
         <f t="shared" si="0"/>
@@ -1911,6 +2343,44 @@
       <c r="G44" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1937,18 +2407,18 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>70</v>
@@ -1959,7 +2429,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>2.8</v>
@@ -1970,7 +2440,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11">
         <f>(B3/60)*0.4571*0.1</f>
@@ -1979,7 +2449,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <f>(H3/60)*(31/90)</f>
@@ -1988,20 +2458,20 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ballast/hull drawings, new servo shaft assy, updated cost breakdown
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B547E6-812F-4F08-BA14-BF1DAE358EFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A8BEBF-7157-4C2D-8803-B9D36159C29C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="164">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -239,9 +239,6 @@
     <t>estimated. Might be able to use an old one</t>
   </si>
   <si>
-    <t>Motor countroller</t>
-  </si>
-  <si>
     <t>.125" ID Bushing</t>
   </si>
   <si>
@@ -461,9 +458,6 @@
     <t>Tether Wire</t>
   </si>
   <si>
-    <t>Radio Equipment</t>
-  </si>
-  <si>
     <t>Any additional Mini Sub Stuff</t>
   </si>
   <si>
@@ -477,6 +471,54 @@
   </si>
   <si>
     <t>QUICRUN 1060 ESC</t>
+  </si>
+  <si>
+    <t>Polycarbonate Tube</t>
+  </si>
+  <si>
+    <t>Motor controller</t>
+  </si>
+  <si>
+    <t>UHMW Ballast Tank Tube, 6" length</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#1988T16</t>
+  </si>
+  <si>
+    <t>https://www.plastic-craft.com/products/pcroundtube?variant=11646907457</t>
+  </si>
+  <si>
+    <t>shipping and cutting cost estimated</t>
+  </si>
+  <si>
+    <t>Total Project Cost:</t>
+  </si>
+  <si>
+    <t>Xbee Pro 80mW Series 1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/XBee-Pro-60mW-Wire-Antenna/dp/B00MYK107Q/ref=cm_cr_arp_d_product_top?ie=UTF8</t>
+  </si>
+  <si>
+    <t>AKK Video Transmitter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AKK-5-8Ghz-Switchable-Transmitter-Pigtail/dp/B01N948FF7/ref=sr_1_9?ie=UTF8&amp;qid=1530481482&amp;sr=8-9&amp;keywords=fpv%2Btransmitter&amp;th=1#customerReviews</t>
+  </si>
+  <si>
+    <t>Have Antenna, don't know if it will work though</t>
+  </si>
+  <si>
+    <t>AKK Video Receiver</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AKK-Receiver-Double-screen-Display-Quadcopter/dp/B01FXFZ0NS/ref=sr_1_13?ie=UTF8&amp;qid=1530481913&amp;sr=8-13&amp;keywords=5.8ghz+video+receiver#customerReviews</t>
+  </si>
+  <si>
+    <t>lipo charger</t>
+  </si>
+  <si>
+    <t>Engel Projected Subtotal:</t>
   </si>
 </sst>
 </file>
@@ -486,7 +528,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,6 +551,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -527,11 +577,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -543,9 +594,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -969,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -1217,24 +1270,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
@@ -1243,7 +1298,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -1269,14 +1324,21 @@
         <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(G3:G68)</f>
-        <v>435.52000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>668.15000000000009</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="2">
+        <f>252.14+J2</f>
+        <v>920.29000000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1305,7 +1367,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1319,21 +1381,21 @@
         <v>8.31</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E44" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E45" si="0">D4*C4</f>
         <v>8.31</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G44" si="1">F4+E4</f>
+        <f t="shared" ref="G4:G45" si="1">F4+E4</f>
         <v>11.31</v>
       </c>
       <c r="H4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1358,7 +1420,7 @@
         <v>6.26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1386,7 +1448,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1414,7 +1476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1442,7 +1504,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1470,7 +1532,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1498,7 +1560,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1526,7 +1588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1546,10 +1608,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1577,11 +1639,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C14">
@@ -1605,11 +1667,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C15">
@@ -1633,7 +1695,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1660,7 +1722,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1685,10 +1747,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
         <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1708,15 +1770,15 @@
         <v>8.77</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1736,15 +1798,15 @@
         <v>1.88</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
         <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1769,10 +1831,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1792,15 +1854,15 @@
         <v>17.16</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
         <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1825,10 +1887,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1853,10 +1915,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
         <v>98</v>
-      </c>
-      <c r="B24" t="s">
-        <v>99</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1881,7 +1943,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25">
         <v>16</v>
@@ -1899,10 +1961,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1927,10 +1989,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1955,440 +2017,537 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>3.56</v>
+        <v>32.630000000000003</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>7.12</v>
+        <v>32.630000000000003</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>7.12</v>
+        <v>36.630000000000003</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>5.12</v>
+        <v>3.56</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
-        <v>15.36</v>
+        <f t="shared" ref="E29:E41" si="2">D29*C29</f>
+        <v>7.12</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>15.36</v>
+        <f t="shared" ref="G29:G41" si="3">F29+E29</f>
+        <v>7.12</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B30" t="s">
+        <v>109</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <v>5.12</v>
+      </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>15.36</v>
+      </c>
+      <c r="F30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="1"/>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>15.36</v>
+      </c>
+      <c r="H30" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0.96</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
-        <v>1.92</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2.5</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>4.42</v>
-      </c>
-      <c r="H31" t="s">
-        <v>44</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>9.49</v>
+        <v>0.96</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
-        <v>9.49</v>
+        <f t="shared" si="2"/>
+        <v>1.92</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>9.49</v>
+        <f t="shared" si="3"/>
+        <v>4.42</v>
       </c>
       <c r="H32" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>21.76</v>
+        <v>9.49</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
-        <v>21.76</v>
+        <f t="shared" si="2"/>
+        <v>9.49</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>21.76</v>
+        <f t="shared" si="3"/>
+        <v>9.49</v>
       </c>
       <c r="H33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>6.99</v>
+        <v>21.76</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
-        <v>6.99</v>
+        <f t="shared" si="2"/>
+        <v>21.76</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>6.99</v>
+        <f t="shared" si="3"/>
+        <v>21.76</v>
       </c>
       <c r="H34" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" s="1">
-        <v>20</v>
+        <v>6.99</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F35" s="1"/>
+        <f t="shared" si="2"/>
+        <v>6.99</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>6.99</v>
       </c>
       <c r="H35" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" s="1">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" s="1">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="2">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" si="3"/>
+        <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" s="1">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
       <c r="H39" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>19</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="H40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
         <v>139</v>
       </c>
-      <c r="B40" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
         <v>7.86</v>
       </c>
-      <c r="E40" s="1">
-        <f t="shared" si="0"/>
+      <c r="E41" s="1">
+        <f t="shared" si="2"/>
         <v>7.86</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F41" s="1">
         <v>3</v>
       </c>
-      <c r="G40" s="2">
-        <f t="shared" si="1"/>
+      <c r="G41" s="2">
+        <f t="shared" si="3"/>
         <v>10.86</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="1"/>
-      <c r="E41" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="1"/>
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>60</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="F42" s="1">
+        <v>20</v>
+      </c>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="H42" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D43" s="1"/>
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>40</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F43" s="1">
         <v>0</v>
       </c>
-      <c r="F43" s="1"/>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="1"/>
+      <c r="A44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>18</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="F44" s="1"/>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <v>18</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52" t="s">
+        <v>162</v>
+      </c>
+      <c r="H52" t="s">
+        <v>163</v>
+      </c>
+      <c r="I52" s="2">
+        <f>G7+G10+G11+G13+G14+G15</f>
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
         <v>141</v>
       </c>
-      <c r="F52" t="s">
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F53" t="s">
+    <row r="57" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F54" t="s">
+    <row r="58" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F55" t="s">
+    <row r="59" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F56" t="s">
+    <row r="60" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="F58" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{5D118521-09C4-4C0E-9CEC-B7FBF6A1D7FB}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{9571E39A-CBF7-4AA2-9D6D-355995927F3A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2407,18 +2566,18 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <v>70</v>
@@ -2429,7 +2588,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>2.8</v>
@@ -2440,7 +2599,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11">
         <f>(B3/60)*0.4571*0.1</f>
@@ -2449,7 +2608,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12">
         <f>(H3/60)*(31/90)</f>
@@ -2458,20 +2617,20 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sweet ballast tank layout and fixturing tools
Lays out and fixtures the UHMW ballast tank for milling.
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A8BEBF-7157-4C2D-8803-B9D36159C29C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F149FD-F7E7-440D-B1F7-41A0BE747A3A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="156">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -176,12 +176,6 @@
     <t>https://www.mcmaster.com/#6658k64/=1dewj1f</t>
   </si>
   <si>
-    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Rudder-Yoke-L5.html</t>
-  </si>
-  <si>
-    <t>Control Yokes 3mm</t>
-  </si>
-  <si>
     <t>300mm long 2mm diameter threaded push rods (2 pack)</t>
   </si>
   <si>
@@ -200,39 +194,9 @@
     <t>Need to check push rod thread for compatibility</t>
   </si>
   <si>
-    <t>Push Rod Seals, 2mm</t>
-  </si>
-  <si>
-    <t>Push Rod Seals, 3mm</t>
-  </si>
-  <si>
-    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Pushrod-Seals/Pushrod-Seal-2-mm.html?listtype=search&amp;searchparam=push</t>
-  </si>
-  <si>
-    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Pushrod-Seals/Pushrod-Seal-3-mm.html</t>
-  </si>
-  <si>
     <t>Bolt, Button Head, 5-40 thread, 1inch long</t>
   </si>
   <si>
-    <t>4mm shaft seal</t>
-  </si>
-  <si>
-    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Shaft-Sealing-Ring-4-11-6-for-shaft-4mm.html?listtype=search&amp;searchparam=seal</t>
-  </si>
-  <si>
-    <t>540 Motor Mount</t>
-  </si>
-  <si>
-    <t>http://engel-modellbau.eu/shop/en/Sub-Components/Spare-Parts/Motor-Mount-540.html</t>
-  </si>
-  <si>
-    <t>http://engel-modellbau.eu/shop/en/Ship/Accessories/Couplings/Coupler-3-17-4mm.html</t>
-  </si>
-  <si>
-    <t>Motor Coupling</t>
-  </si>
-  <si>
     <t>DC Motor 80T</t>
   </si>
   <si>
@@ -518,7 +482,19 @@
     <t>lipo charger</t>
   </si>
   <si>
-    <t>Engel Projected Subtotal:</t>
+    <t>Engel Order</t>
+  </si>
+  <si>
+    <t>Shaft seal, motor mount, coupler, rod seals, yokes</t>
+  </si>
+  <si>
+    <t>Engel</t>
+  </si>
+  <si>
+    <t>Epoxy Coating Tools</t>
+  </si>
+  <si>
+    <t>100 pack medicine cups, assorted paintbrushes</t>
   </si>
 </sst>
 </file>
@@ -591,10 +567,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -913,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7607A2C9-437F-4FE2-AFDA-0D0C0CE9A3E2}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,17 +903,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -960,7 +936,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(E3:E39)</f>
-        <v>252.14</v>
+        <v>356.95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1022,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -1133,17 +1109,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="1"/>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>43290</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="1">
+        <v>92.31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43295</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
@@ -1272,14 +1270,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
@@ -1287,16 +1285,17 @@
     <col min="8" max="8" width="33.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1324,18 +1323,18 @@
         <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(G3:G68)</f>
-        <v>668.15000000000009</v>
+        <v>568.65</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="M2" s="2">
-        <f>252.14+J2</f>
-        <v>920.29000000000008</v>
+        <f>344.45+J2</f>
+        <v>913.09999999999991</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1449,39 +1448,17 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>40.5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>45.5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1501,15 +1478,15 @@
         <v>4.99</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1529,68 +1506,24 @@
         <v>4.63</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1608,96 +1541,32 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H13" t="s">
-        <v>44</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="H14" t="s">
-        <v>44</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1717,12 +1586,12 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1742,15 +1611,15 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1770,15 +1639,15 @@
         <v>8.77</v>
       </c>
       <c r="H18" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1798,15 +1667,15 @@
         <v>1.88</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -1831,10 +1700,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>74</v>
+        <v>60</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1854,15 +1723,15 @@
         <v>17.16</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -1887,10 +1756,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1915,10 +1784,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1943,7 +1812,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C25">
         <v>16</v>
@@ -1961,10 +1830,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1989,10 +1858,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2017,10 +1886,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2045,10 +1914,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2068,15 +1937,15 @@
         <v>7.12</v>
       </c>
       <c r="H29" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -2096,12 +1965,12 @@
         <v>15.36</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -2119,10 +1988,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2147,10 +2016,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2170,15 +2039,15 @@
         <v>9.49</v>
       </c>
       <c r="H33" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2198,15 +2067,15 @@
         <v>21.76</v>
       </c>
       <c r="H34" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2226,15 +2095,15 @@
         <v>6.99</v>
       </c>
       <c r="H35" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2252,15 +2121,15 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2278,15 +2147,15 @@
         <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2304,15 +2173,15 @@
         <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2330,15 +2199,15 @@
         <v>27</v>
       </c>
       <c r="H39" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2356,15 +2225,15 @@
         <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2389,10 +2258,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2412,15 +2281,15 @@
         <v>80</v>
       </c>
       <c r="H42" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -2442,10 +2311,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2465,15 +2334,15 @@
         <v>18</v>
       </c>
       <c r="H44" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2495,47 +2364,41 @@
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F52" t="s">
-        <v>162</v>
-      </c>
-      <c r="H52" t="s">
-        <v>163</v>
-      </c>
-      <c r="I52" s="2">
-        <f>G7+G10+G11+G13+G14+G15</f>
-        <v>99.5</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I52" s="2"/>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2543,11 +2406,10 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{5D118521-09C4-4C0E-9CEC-B7FBF6A1D7FB}"/>
-    <hyperlink ref="B15" r:id="rId2" xr:uid="{9571E39A-CBF7-4AA2-9D6D-355995927F3A}"/>
+    <hyperlink ref="B21" r:id="rId1" location="1257k39/=1dfcnqq" xr:uid="{1885B411-AD7F-4768-BF83-5734B2F35F56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2566,18 +2428,18 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>70</v>
@@ -2588,7 +2450,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>2.8</v>
@@ -2599,7 +2461,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B11">
         <f>(B3/60)*0.4571*0.1</f>
@@ -2608,7 +2470,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H12">
         <f>(H3/60)*(31/90)</f>
@@ -2617,20 +2479,20 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Rods, Added list of machine work left to be done
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E95A57D-659E-43E7-A339-205F6B1CFD14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8000B801-D5C2-4253-A717-9DA038732CDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -938,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7607A2C9-437F-4FE2-AFDA-0D0C0CE9A3E2}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,14 +1959,14 @@
         <v>3.56</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" ref="E21:E33" si="4">D21*C21</f>
+        <f t="shared" ref="E21:E22" si="4">D21*C21</f>
         <v>7.12</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ref="G21:G33" si="5">F21+E21</f>
+        <f t="shared" ref="G21:G22" si="5">F21+E21</f>
         <v>7.12</v>
       </c>
       <c r="H21" t="s">
@@ -2015,14 +2015,14 @@
         <v>0.96</v>
       </c>
       <c r="E23" s="1">
-        <f>D23*C23</f>
+        <f t="shared" ref="E23:E39" si="6">D23*C23</f>
         <v>1.92</v>
       </c>
       <c r="F23" s="1">
         <v>2.5</v>
       </c>
       <c r="G23" s="2">
-        <f>F23+E23</f>
+        <f t="shared" ref="G23:G39" si="7">F23+E23</f>
         <v>4.42</v>
       </c>
       <c r="H23" t="s">
@@ -2043,14 +2043,14 @@
         <v>9.49</v>
       </c>
       <c r="E24" s="1">
-        <f>D24*C24</f>
+        <f t="shared" si="6"/>
         <v>9.49</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
       <c r="G24" s="2">
-        <f>F24+E24</f>
+        <f t="shared" si="7"/>
         <v>9.49</v>
       </c>
       <c r="H24" t="s">
@@ -2071,14 +2071,14 @@
         <v>21.76</v>
       </c>
       <c r="E25" s="1">
-        <f>D25*C25</f>
+        <f t="shared" si="6"/>
         <v>21.76</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
       </c>
       <c r="G25" s="2">
-        <f>F25+E25</f>
+        <f t="shared" si="7"/>
         <v>21.76</v>
       </c>
       <c r="H25" t="s">
@@ -2099,14 +2099,14 @@
         <v>6.99</v>
       </c>
       <c r="E26" s="1">
-        <f>D26*C26</f>
+        <f t="shared" si="6"/>
         <v>6.99</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <f>F26+E26</f>
+        <f t="shared" si="7"/>
         <v>6.99</v>
       </c>
       <c r="H26" t="s">
@@ -2127,12 +2127,12 @@
         <v>20</v>
       </c>
       <c r="E27" s="1">
-        <f>D27*C27</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2">
-        <f>F27+E27</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H27" t="s">
@@ -2156,12 +2156,12 @@
         <v>10</v>
       </c>
       <c r="E28" s="1">
-        <f>D28*C28</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="2">
-        <f>F28+E28</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="H28" t="s">
@@ -2185,12 +2185,12 @@
         <v>44</v>
       </c>
       <c r="E29" s="1">
-        <f>D29*C29</f>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="2">
-        <f>F29+E29</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="H29" t="s">
@@ -2214,12 +2214,12 @@
         <v>27</v>
       </c>
       <c r="E30" s="1">
-        <f>D30*C30</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="2">
-        <f>F30+E30</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="H30" t="s">
@@ -2243,12 +2243,12 @@
         <v>19</v>
       </c>
       <c r="E31" s="1">
-        <f>D31*C31</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="2">
-        <f>F31+E31</f>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="H31" t="s">
@@ -2272,14 +2272,14 @@
         <v>7.86</v>
       </c>
       <c r="E32" s="1">
-        <f>D32*C32</f>
+        <f t="shared" si="6"/>
         <v>7.86</v>
       </c>
       <c r="F32" s="1">
         <v>3</v>
       </c>
       <c r="G32" s="2">
-        <f>F32+E32</f>
+        <f t="shared" si="7"/>
         <v>10.86</v>
       </c>
       <c r="H32" t="s">
@@ -2300,14 +2300,14 @@
         <v>17</v>
       </c>
       <c r="E33" s="1">
-        <f>D33*C33</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f>F33+E33</f>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
     </row>
@@ -2325,14 +2325,14 @@
         <v>18</v>
       </c>
       <c r="E34" s="1">
-        <f>D34*C34</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f>F34+E34</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
     </row>
@@ -2350,14 +2350,14 @@
         <v>18</v>
       </c>
       <c r="E35" s="1">
-        <f>D35*C35</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f>F35+E35</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="I35" s="3" t="s">
@@ -2378,14 +2378,14 @@
         <v>6.71</v>
       </c>
       <c r="E36" s="1">
-        <f>D36*C36</f>
+        <f t="shared" si="6"/>
         <v>6.71</v>
       </c>
       <c r="F36" s="1">
         <v>3</v>
       </c>
       <c r="G36" s="2">
-        <f>F36+E36</f>
+        <f t="shared" si="7"/>
         <v>9.7100000000000009</v>
       </c>
       <c r="H36" t="s">
@@ -2406,14 +2406,14 @@
         <v>1.62</v>
       </c>
       <c r="E37" s="1">
-        <f>D37*C37</f>
+        <f t="shared" si="6"/>
         <v>1.62</v>
       </c>
       <c r="F37" s="1">
         <v>2</v>
       </c>
       <c r="G37" s="2">
-        <f>F37+E37</f>
+        <f t="shared" si="7"/>
         <v>3.62</v>
       </c>
       <c r="H37" t="s">
@@ -2434,14 +2434,14 @@
         <v>8</v>
       </c>
       <c r="E38" s="1">
-        <f>D38*C38</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f>F38+E38</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
@@ -2459,14 +2459,14 @@
         <v>2.09</v>
       </c>
       <c r="E39" s="1">
-        <f>D39*C39</f>
+        <f t="shared" si="6"/>
         <v>2.09</v>
       </c>
       <c r="F39" s="1">
         <v>3</v>
       </c>
       <c r="G39" s="2">
-        <f>F39+E39</f>
+        <f t="shared" si="7"/>
         <v>5.09</v>
       </c>
       <c r="H39" t="s">

</xml_diff>

<commit_message>
sail and hall effect sensor mount updates
</commit_message>
<xml_diff>
--- a/Docs/Cost Breakdown.xlsx
+++ b/Docs/Cost Breakdown.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Submarine\Submarine-project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8000B801-D5C2-4253-A717-9DA038732CDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1044AF1-1365-452B-98E9-EA0999AC0926}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F21002F-912E-4475-A97C-0E0680C7FAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="SERVO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>Submarine Cost Breakdown</t>
   </si>
@@ -137,75 +137,12 @@
     <t>Add. Notes</t>
   </si>
   <si>
-    <t>4mm Ball Bearing</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#7804k129/=1dew8kd</t>
-  </si>
-  <si>
     <t>Shipping</t>
   </si>
   <si>
     <t>Total Price W/O Shipping</t>
   </si>
   <si>
-    <t>shipping estimated.</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Airplane-Stainless-Steel-Round-Axles/dp/B00OK42ZOG/ref=sr_1_10?ie=UTF8&amp;qid=1529786532&amp;sr=8-10&amp;keywords=3mm+shaft</t>
-  </si>
-  <si>
-    <t>3mm shaft (5pack) for all control surfaces</t>
-  </si>
-  <si>
-    <t>3mm bushings</t>
-  </si>
-  <si>
-    <t>300mm long 2mm diameter threaded push rods (2 pack)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/uxcell-Airplane-Parts-Threaded-Length/dp/B01LBJKQZW/ref=sr_1_47?ie=UTF8&amp;qid=1529789116&amp;sr=8-47&amp;keywords=2mm+rod</t>
-  </si>
-  <si>
-    <t>Thread class unknown</t>
-  </si>
-  <si>
-    <t>2mm clevises (pack of 5)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Threaded-Metal-Clevis-2x25mm-Airplane/dp/B00XBGKIKC/ref=sr_1_3?ie=UTF8&amp;qid=1529788008&amp;sr=8-3&amp;keywords=clevis+2mm&amp;dpID=41IfImQMKkL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>Need to check push rod thread for compatibility</t>
-  </si>
-  <si>
-    <t>Bolt, Button Head, 5-40 thread, 1inch long</t>
-  </si>
-  <si>
-    <t>DC Motor 80T</t>
-  </si>
-  <si>
-    <t>.125" ID Bushing</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#6391k113/=1dey23w</t>
-  </si>
-  <si>
-    <t>.125" shaft</t>
-  </si>
-  <si>
-    <t>need 22 inches total</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#1257k39/=1dfcnqq</t>
-  </si>
-  <si>
-    <t>Encoder magnets</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#5862k13/=1cd8mhi</t>
-  </si>
-  <si>
     <t>HS 82MG</t>
   </si>
   <si>
@@ -239,105 +176,6 @@
     <t>https://www.amazon.com/SODIAL-Aluminum-Flexible-Coupling-Connector/dp/B072KRCMJS/ref=sr_1_10?s=hi&amp;ie=UTF8&amp;qid=1529867349&amp;sr=1-10&amp;keywords=3mm%2Bshaft%2Bcoupler&amp;th=1</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#6391k126/=1dfi0m4</t>
-  </si>
-  <si>
-    <t>.25" bushings</t>
-  </si>
-  <si>
-    <t>.25" diameter 5" long spool shaft</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#1257k115/=1dfi12u</t>
-  </si>
-  <si>
-    <t>Bolt, Button Head, 5-40 thread, .625" long</t>
-  </si>
-  <si>
-    <t>Could also use .875"</t>
-  </si>
-  <si>
-    <t>Ballast Tank Threaded Rod (5/16-18 thread)</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#90611a400/=1dfi2y2</t>
-  </si>
-  <si>
-    <t>Screw-Mount Nut (5/16-18) For Ballast Tank (25count)</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#98752a523/=1dfi7du</t>
-  </si>
-  <si>
-    <t>28T Pinion Gear (2count)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/TOOGOO-3-175mm-Pinion-Brushed-Brushless/dp/B075FN58G6/ref=sr_1_54?ie=UTF8&amp;qid=1529888786&amp;sr=8-54&amp;keywords=28t+pinion+gear</t>
-  </si>
-  <si>
-    <t>Long Shipping time</t>
-  </si>
-  <si>
-    <t>16T Pinion Gear 48P</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Traxxas-2416-16T-Pinion-Gear/dp/B000XQ2KTU/ref=sr_1_4?ie=UTF8&amp;qid=1529889119&amp;sr=8-4&amp;keywords=16T+pinion+gear+set</t>
-  </si>
-  <si>
-    <t>Check Other sites for better pricing (bulk)</t>
-  </si>
-  <si>
-    <t>Ballast Thrust Bearing</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#5906k513/=1cyvllx</t>
-  </si>
-  <si>
-    <t>.125" Bearing (.25" OD, 10 count)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/125x-250x-109-Precision-Bearings-Metal-Shields/dp/B00X8KXAFG/ref=sr_1_4?ie=UTF8&amp;qid=1523395530&amp;sr=8-4&amp;keywords=ball+bearings+1%2F8+1%2F4&amp;dpID=41aeoNIanLL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>For Ballast Gear Train, Spool Carriage Threaded Rod</t>
-  </si>
-  <si>
-    <t>5V 10A Buck Converter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Castle-Creations-Bec-Switching-Regulator/dp/B000MXAR12/ref=sr_1_1?ie=UTF8&amp;qid=1529889704&amp;sr=8-1&amp;keywords=BEC+10A</t>
-  </si>
-  <si>
-    <t>Maybe find one cheaper? Need 10A though</t>
-  </si>
-  <si>
-    <t>16 Channel PWM Driver</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/HiLetgo-PCA9685-Channel-12-Bit-Arduino/dp/B01D1D0CX2/ref=sr_1_2?ie=UTF8&amp;qid=1529890412&amp;sr=8-2&amp;keywords=servo+driver+board&amp;dpID=511228KD6JL&amp;preST=_SY300_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>For all PWM (servos, LEDs, etc)</t>
-  </si>
-  <si>
-    <t>Arduino Nano 5 Pack</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B01N7I0W77/ref=sxbs_sxwds-stppvp_3?pf_rd_m=ATVPDKIKX0DER&amp;pf_rd_p=6297546923292665688&amp;pd_rd_wg=ddHdE&amp;pf_rd_r=SXBWPAFRVYFKDFR5S237&amp;pf_rd_s=desktop-sx-bottom-slot&amp;pf_rd_t=301&amp;pd_rd_i=B01N7I0W77&amp;pd_rd_w=GY6XU&amp;pf_rd_i=arduino+nano+5+pack&amp;pd_rd_r=3a7c9f18-fd3d-491b-86c9-19ec55cea102&amp;ie=UTF8&amp;qid=1529890713&amp;sr=3#customerReviews</t>
-  </si>
-  <si>
-    <t>Look around for better bulk pricing if need be (unsoldered only)</t>
-  </si>
-  <si>
-    <t>5V Relay 5 Pack</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/WINGONEER-KY-019-Channel-Module-arduino/dp/B06XHJ2PBJ/ref=sr_1_3?ie=UTF8&amp;qid=1529890983&amp;sr=8-3&amp;keywords=5V+relay&amp;dpID=51AfIoxmEZL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>Maybe don't need, use existing relays with BJT circuit</t>
-  </si>
-  <si>
     <t>11.1V Drive Battery 5500mAh</t>
   </si>
   <si>
@@ -365,12 +203,6 @@
     <t>Check before ordering</t>
   </si>
   <si>
-    <t>Electronics Battery Oring</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#9557k134/=1bkj08p</t>
-  </si>
-  <si>
     <t>NOT INCLUDED SO FAR:</t>
   </si>
   <si>
@@ -392,12 +224,6 @@
     <t>QUICRUN 1060 ESC</t>
   </si>
   <si>
-    <t>AKK Video Transmitter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/AKK-5-8Ghz-Switchable-Transmitter-Pigtail/dp/B01N948FF7/ref=sr_1_9?ie=UTF8&amp;qid=1530481482&amp;sr=8-9&amp;keywords=fpv%2Btransmitter&amp;th=1#customerReviews</t>
-  </si>
-  <si>
     <t>AKK Video Receiver</t>
   </si>
   <si>
@@ -452,12 +278,6 @@
     <t>Need to test</t>
   </si>
   <si>
-    <t>https://www.amazon.com/MakerFocus-NRF24L01-Transceiver-Antistatic-Compatible/dp/B07BNDKFXP/ref=pd_sim_23_31?_encoding=UTF8&amp;pd_rd_i=B01IK78PQA&amp;pd_rd_r=5e913b3d-87b0-11e8-a387-cb55ff1621b3&amp;pd_rd_w=no0NJ&amp;pd_rd_wg=4eoml&amp;pf_rd_i=desktop-dp-sims&amp;pf_rd_m=ATVPDKIKX0DER&amp;pf_rd_p=7967298517161621930&amp;pf_rd_r=CX9Z951BFW3QA0MHWY35&amp;pf_rd_s=desktop-dp-sims&amp;pf_rd_t=40701&amp;refRID=CX9Z951BFW3QA0MHWY35&amp;th=1</t>
-  </si>
-  <si>
-    <t>nRF24L01P 2x SPI 100mW transceivers + SMA 2db Antennas</t>
-  </si>
-  <si>
     <t>Polycarb Tube</t>
   </si>
   <si>
@@ -467,42 +287,6 @@
     <t>Plastic-Craft</t>
   </si>
   <si>
-    <t>tether wire extension ($10)</t>
-  </si>
-  <si>
-    <t>New Primary o Rings</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#1302n55/=1dt71oi</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#6659k64/=1dt9z76</t>
-  </si>
-  <si>
-    <t>Aluminum ballast tube</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#9056k41/=1dta0ei</t>
-  </si>
-  <si>
-    <t>PTFE film</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#8569k12/=1dtavdo</t>
-  </si>
-  <si>
-    <t>electromagnet</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/uxcell-Electric-Lifting-Electromagnet-Solenoid/dp/B01N3387AA/ref=sr_1_5?ie=UTF8&amp;qid=1532203628&amp;sr=8-5&amp;keywords=electromagnet&amp;dpID=41UfKlt5MDL&amp;preST=_SY300_QL70_&amp;dpSrc=srch&amp;th=1</t>
-  </si>
-  <si>
-    <t>holding magnet, minisub</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#5862k12/=1dtaz6c</t>
-  </si>
-  <si>
     <t>ServoCity</t>
   </si>
   <si>
@@ -512,15 +296,6 @@
     <t>Drive Shaft</t>
   </si>
   <si>
-    <t>https://www.amazon.com/RC4WD-540-Crawler-Brushed-Motor/dp/B00CR32LZ0/ref=sr_1_2?ie=UTF8&amp;qid=1532207826&amp;sr=8-2&amp;keywords=540+80T&amp;dpID=4119R2Lh9yL&amp;preST=_SX300_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/HobbyWing-QUICRUN-1060-Brushed-ESC/dp/B00LXCM3Q8/ref=sr_1_2?ie=UTF8&amp;qid=1532207875&amp;sr=8-2&amp;keywords=quicrun+1060&amp;dpID=41wM%252Bd2dDqL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
-  </si>
-  <si>
-    <t>Quicrun 1060 ESC</t>
-  </si>
-  <si>
     <t>2x 16T Pinion Gears</t>
   </si>
   <si>
@@ -542,7 +317,10 @@
     <t>4mm BB, 2x .25 bushing, 11x .125 bushing, 2x .125 shaft, 11x micro magnets, 4x flanged 3mm bushing, .25 shaft, 5/16-18 threaded rod 1ft, 5/16-18 screw-mount nuts, Al6061 ballast tube, 2x ballast thrust bearings, electronics battery O rings, new primary sealing orings, teflon film, minisub magnet</t>
   </si>
   <si>
-    <t xml:space="preserve">MERCHANDISE ONLY. ADD SHIPPING WHEN BILLED. </t>
+    <t>Amazon order</t>
+  </si>
+  <si>
+    <t>wires, relays, loctite, arduinos</t>
   </si>
 </sst>
 </file>
@@ -938,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7607A2C9-437F-4FE2-AFDA-0D0C0CE9A3E2}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,14 +760,14 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="I2" s="2">
         <f>SUM(E3:E39)</f>
-        <v>675.6099999999999</v>
+        <v>761.90999999999985</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1051,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -1167,10 +945,10 @@
         <v>43277</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>8</v>
@@ -1179,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1187,13 +965,13 @@
         <v>43290</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="E14" s="1">
         <v>92.31</v>
@@ -1204,10 +982,10 @@
         <v>43295</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>8</v>
@@ -1221,10 +999,10 @@
         <v>43295</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>8</v>
@@ -1233,7 +1011,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1241,13 +1019,13 @@
         <v>43300</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1">
         <v>50.45</v>
@@ -1258,13 +1036,13 @@
         <v>43302</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="E18" s="1">
         <v>8.08</v>
@@ -1275,13 +1053,13 @@
         <v>43302</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="E19" s="1">
         <v>6.37</v>
@@ -1292,10 +1070,10 @@
         <v>43302</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -1309,26 +1087,35 @@
         <v>43302</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>169</v>
+        <v>94</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="1">
-        <v>92.76</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="4">
+        <v>43311</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
+        <v>40.06</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
@@ -1409,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B288EA7B-40F8-4459-809C-4DF58A54F923}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,10 +1238,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>33</v>
@@ -1463,11 +1250,11 @@
         <v>35</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="L2" s="2">
         <f>SUM(G3:G68)</f>
-        <v>412.94999999999993</v>
+        <v>108</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="2"/>
@@ -1479,704 +1266,179 @@
       <c r="G3" s="2"/>
       <c r="I3" s="2"/>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="L3" s="7">
         <f>Sheet1!I2</f>
-        <v>675.6099999999999</v>
+        <v>761.90999999999985</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8.31</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" ref="E4:E6" si="0">D4*C4</f>
-        <v>8.31</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G6" si="1">F4+E4</f>
-        <v>11.31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
       <c r="K4" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="L4" s="2">
         <f>L2+L3</f>
-        <v>1088.56</v>
+        <v>869.90999999999985</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>6.26</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>6.26</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="1"/>
-        <v>6.26</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.71</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>6.84</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="1"/>
-        <v>9.84</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" ref="E7:E20" si="2">D7*C7</f>
-        <v>4.99</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" ref="G7:G20" si="3">F7+E7</f>
-        <v>4.99</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4.63</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>4.63</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="3"/>
-        <v>4.63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>49</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>75</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>11.88</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>11.88</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="3"/>
-        <v>11.88</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>20.99</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>20.99</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="3"/>
-        <v>20.99</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>5.6000000000000005</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="3"/>
-        <v>7.6000000000000005</v>
-      </c>
-      <c r="H12" t="s">
-        <v>40</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>6.58</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>13.16</v>
-      </c>
-      <c r="F13" s="1">
-        <v>4</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="3"/>
-        <v>17.16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>55</v>
-      </c>
+      <c r="B13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.48</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>4.8</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="3"/>
-        <v>6.8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.86</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="3"/>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="H15" t="s">
-        <v>40</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5.01</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>5.01</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="3"/>
-        <v>6.51</v>
-      </c>
-      <c r="H16" t="s">
-        <v>40</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="F18" s="1">
-        <v>3</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="3"/>
-        <v>7.98</v>
-      </c>
-      <c r="H18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>7.77</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>7.77</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="3"/>
-        <v>9.77</v>
-      </c>
-      <c r="H19" t="s">
-        <v>40</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>14.19</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>14.19</v>
-      </c>
-      <c r="F20" s="1">
-        <v>6</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="3"/>
-        <v>20.189999999999998</v>
-      </c>
-      <c r="H20" t="s">
-        <v>40</v>
-      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3.56</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" ref="E21:E22" si="4">D21*C21</f>
-        <v>7.12</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" ref="G21:G22" si="5">F21+E21</f>
-        <v>7.12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>82</v>
-      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5.12</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="4"/>
-        <v>5.12</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="5"/>
-        <v>5.12</v>
-      </c>
-      <c r="H22" t="s">
-        <v>85</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.96</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" ref="E23:E39" si="6">D23*C23</f>
-        <v>1.92</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" ref="G23:G39" si="7">F23+E23</f>
-        <v>4.42</v>
-      </c>
-      <c r="H23" t="s">
-        <v>40</v>
-      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>9.49</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="6"/>
-        <v>9.49</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="7"/>
-        <v>9.49</v>
-      </c>
-      <c r="H24" t="s">
-        <v>90</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>21.76</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="6"/>
-        <v>21.76</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="7"/>
-        <v>21.76</v>
-      </c>
-      <c r="H25" t="s">
-        <v>93</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="6"/>
-        <v>6.99</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="7"/>
-        <v>6.99</v>
-      </c>
-      <c r="H26" t="s">
-        <v>96</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>20</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="2">
-        <f t="shared" si="7"/>
-        <v>20</v>
-      </c>
-      <c r="H27" t="s">
-        <v>99</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>166</v>
-      </c>
+      <c r="G27" s="2"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="2">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="H28" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>166</v>
-      </c>
+      <c r="G28" s="2"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2185,27 +1447,27 @@
         <v>44</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E23:E39" si="0">D29*C29</f>
         <v>44</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="G23:G39" si="1">F29+E29</f>
         <v>44</v>
       </c>
       <c r="H29" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2214,27 +1476,27 @@
         <v>27</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2243,105 +1505,45 @@
         <v>19</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H31" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>7.86</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="6"/>
-        <v>7.86</v>
-      </c>
-      <c r="F32" s="1">
-        <v>3</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="7"/>
-        <v>10.86</v>
-      </c>
-      <c r="H32" t="s">
-        <v>40</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>17</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="6"/>
-        <v>17</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="7"/>
-        <v>17</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B34" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>18</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="7"/>
-        <v>18</v>
-      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2350,177 +1552,84 @@
         <v>18</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
-        <v>6.71</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="6"/>
-        <v>6.71</v>
-      </c>
-      <c r="F36" s="1">
-        <v>3</v>
-      </c>
-      <c r="G36" s="2">
-        <f t="shared" si="7"/>
-        <v>9.7100000000000009</v>
-      </c>
-      <c r="H36" t="s">
-        <v>40</v>
-      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" t="s">
-        <v>153</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="6"/>
-        <v>1.62</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="7"/>
-        <v>3.62</v>
-      </c>
-      <c r="H37" t="s">
-        <v>40</v>
-      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>154</v>
-      </c>
-      <c r="B38" t="s">
-        <v>155</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="6"/>
-        <v>2.09</v>
-      </c>
-      <c r="F39" s="1">
-        <v>3</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="7"/>
-        <v>5.09</v>
-      </c>
-      <c r="H39" t="s">
-        <v>40</v>
-      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="F52" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="I52" s="2"/>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F55" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" location="1257k39/=1dfcnqq" xr:uid="{1885B411-AD7F-4768-BF83-5734B2F35F56}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2539,18 +1648,18 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>70</v>
@@ -2561,7 +1670,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>2.8</v>
@@ -2572,7 +1681,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <f>(B3/60)*0.4571*0.1</f>
@@ -2581,7 +1690,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="H12">
         <f>(H3/60)*(31/90)</f>
@@ -2590,20 +1699,20 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>